<commit_message>
edits and fixing errors in percent
</commit_message>
<xml_diff>
--- a/data-raw/quicksummary.xlsx
+++ b/data-raw/quicksummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dyn4cast\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DA4DEB0-316E-4082-83D5-D3EDFF2B990C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994FC965-C024-49A3-BAC1-B06D81EF7161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AB5E97E9-1D30-4155-9956-08FC413C1CBF}"/>
   </bookViews>
@@ -35,101 +35,107 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
-    <t>Lack of access to adequate finance</t>
+    <t>Likert scores 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Lack of appropriate equipment </t>
+    <t>Likert scores 2</t>
   </si>
   <si>
-    <t>Lack of appropriate maintenance technology of the processing machines</t>
+    <t>Likert scores 3</t>
   </si>
   <si>
-    <t>Poor quality of product</t>
+    <t>Likert scores 4</t>
   </si>
   <si>
-    <t>Lack of price information</t>
+    <t>Likert scores 5</t>
   </si>
   <si>
-    <t>Lack of market information</t>
+    <t>Likert scores 6</t>
   </si>
   <si>
-    <t>Low prices of products</t>
+    <t>Likert scores 7</t>
   </si>
   <si>
-    <t>Inadequate access to local markets</t>
+    <t>Likert scores 8</t>
   </si>
   <si>
-    <t>Inadequate access to international market</t>
+    <t>Likert scores 9</t>
   </si>
   <si>
-    <t>Low bargaining power</t>
+    <t>Likert scores 10</t>
   </si>
   <si>
-    <t>Long distance to source of supply</t>
+    <t>Likert scores 11</t>
   </si>
   <si>
-    <t>Long distance to market</t>
+    <t>Likert scores 12</t>
   </si>
   <si>
-    <t>Inadequate access to processors</t>
+    <t>Likert scores 13</t>
   </si>
   <si>
-    <t>Lack of product quality regulation</t>
+    <t>Likert scores 14</t>
   </si>
   <si>
-    <t>problem with transportation of product</t>
+    <t>Likert scores 15</t>
   </si>
   <si>
-    <t>seasonal/irregular supply of product</t>
+    <t>Likert scores 16</t>
   </si>
   <si>
-    <t>High cost of energy source</t>
+    <t>Likert scores 17</t>
   </si>
   <si>
-    <t>Inadequate supply of water</t>
+    <t>Likert scores 18</t>
   </si>
   <si>
-    <t>Shortage of fuel wood</t>
+    <t>Likert scores 19</t>
   </si>
   <si>
-    <t>High and multiple taxation</t>
+    <t>Likert scores 20</t>
   </si>
   <si>
-    <t>Poor storage facilities</t>
+    <t>Likert scores 21</t>
   </si>
   <si>
-    <t>Body pains</t>
+    <t>Likert scores 22</t>
   </si>
   <si>
-    <t>Insecurity</t>
+    <t>Likert scores 23</t>
   </si>
   <si>
-    <t>felling of trees</t>
+    <t>Likert scores 24</t>
   </si>
   <si>
-    <t>Low yield of trees</t>
+    <t>Likert scores 25</t>
   </si>
   <si>
-    <t>Lack of proper labelling and certification mechanism</t>
+    <t>Likert scores 26</t>
   </si>
   <si>
-    <t>Inadequate access to extension and advisory services</t>
+    <t>Likert scores 27</t>
   </si>
   <si>
-    <t>Exposure to health hazards in handling products</t>
+    <t>Likert scores 28</t>
   </si>
   <si>
-    <t>Lack of training in processing skills</t>
+    <t>Likert scores 29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -473,7 +479,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0B1FD6-F0EC-4637-AEE0-D48A5A120F94}">
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -500,70 +508,70 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
         <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" t="s">
-        <v>15</v>
-      </c>
-      <c r="V1" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
@@ -9734,6 +9742,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>